<commit_message>
Created artifact: JAR file
</commit_message>
<xml_diff>
--- a/src/main/resources/ProviderFiles/HRV/HRV_Template.xlsx
+++ b/src/main/resources/ProviderFiles/HRV/HRV_Template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\ReportKisser\src\main\resources\ProviderFiles\HRV\"/>
     </mc:Choice>
@@ -128,8 +128,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -1042,12 +1042,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.33203125" customWidth="1"/>
-    <col min="2" max="2" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.44140625" customWidth="1"/>
-    <col min="4" max="5" width="21.88671875" customWidth="1"/>
-    <col min="6" max="9" width="20.33203125" customWidth="1"/>
-    <col min="10" max="10" width="22" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="2.33203125"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="23.44140625"/>
+    <col min="3" max="3" customWidth="true" width="23.44140625"/>
+    <col min="4" max="5" customWidth="true" width="21.88671875"/>
+    <col min="6" max="9" customWidth="true" width="20.33203125"/>
+    <col min="10" max="10" customWidth="true" width="22.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
@@ -1323,7 +1323,9 @@
       <c r="B19" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="55"/>
+      <c r="C19" s="55" t="n">
+        <v>88.0</v>
+      </c>
       <c r="D19" s="10">
         <f>IF($C$22&lt;100000,C19,100000*(C19/$C$22))</f>
         <v>0</v>
@@ -1353,7 +1355,9 @@
       <c r="B20" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="55"/>
+      <c r="C20" s="55" t="n">
+        <v>1913.75</v>
+      </c>
       <c r="D20" s="10">
         <f>IF($C$22&lt;100000,C20,100000*(C20/$C$22))</f>
         <v>0</v>
@@ -1431,13 +1435,13 @@
     </row>
     <row r="23" spans="1:19" s="22" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="52"/>
-      <c r="B23"/>
-      <c r="C23"/>
+      <c r="B23" s="0"/>
+      <c r="C23" s="0"/>
       <c r="D23" s="53"/>
       <c r="E23" s="53"/>
-      <c r="F23"/>
-      <c r="G23"/>
-      <c r="I23"/>
+      <c r="F23" s="0"/>
+      <c r="G23" s="0"/>
+      <c r="I23" s="0"/>
       <c r="K23" s="29"/>
     </row>
     <row r="24" spans="1:19" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">

</xml_diff>